<commit_message>
it's seems like i am gonna die
</commit_message>
<xml_diff>
--- a/електрична частна станцій та підстанцій/електрична частна станцій та підстанцій.xlsx
+++ b/електрична частна станцій та підстанцій/електрична частна станцій та підстанцій.xlsx
@@ -409,6 +409,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -426,12 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U88"/>
+  <dimension ref="A2:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,14 +1268,14 @@
       <c r="N3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
       <c r="U3" s="7" t="s">
         <v>57</v>
       </c>
@@ -1322,15 +1322,15 @@
         <f>(H4^2)*$J$3</f>
         <v>1862.2547878524683</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="8"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="10"/>
     </row>
     <row r="5" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1437,7 +1437,7 @@
         <f>(H6^2)*$J$3</f>
         <v>7575.9673647973123</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="8"/>
       <c r="N6" s="5" t="s">
         <v>60</v>
       </c>
@@ -1453,9 +1453,9 @@
       <c r="R6" s="5">
         <v>3.16</v>
       </c>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -1495,7 +1495,7 @@
         <f t="shared" si="4"/>
         <v>11057.127645581084</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="5" t="s">
         <v>61</v>
       </c>
@@ -1511,9 +1511,9 @@
       <c r="R7" s="5">
         <v>3.16</v>
       </c>
-      <c r="S7" s="15"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1553,7 +1553,7 @@
         <f t="shared" si="4"/>
         <v>4719.0488272382081</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="5" t="s">
         <v>62</v>
       </c>
@@ -1572,8 +1572,8 @@
       <c r="S8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1613,7 +1613,7 @@
         <f>(H9^2)*$J$3</f>
         <v>29828.185655256664</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="5" t="s">
         <v>63</v>
       </c>
@@ -1629,9 +1629,9 @@
       <c r="R9" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
     </row>
     <row r="10" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1671,7 +1671,7 @@
         <f>(H10^2)*$J$4</f>
         <v>9787.0709056441628</v>
       </c>
-      <c r="M10" s="15"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="6" t="s">
         <v>64</v>
       </c>
@@ -1799,7 +1799,7 @@
         <f t="shared" si="4"/>
         <v>11057.127645581084</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="5" t="s">
         <v>60</v>
       </c>
@@ -1815,9 +1815,9 @@
       <c r="R12" s="5">
         <v>3.16</v>
       </c>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1857,7 +1857,7 @@
         <f t="shared" si="4"/>
         <v>7575.9673647973123</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="5" t="s">
         <v>61</v>
       </c>
@@ -1873,9 +1873,9 @@
       <c r="R13" s="5">
         <v>3.16</v>
       </c>
-      <c r="S13" s="15"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1915,7 +1915,7 @@
         <f t="shared" si="4"/>
         <v>4719.0488272382081</v>
       </c>
-      <c r="M14" s="14"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1934,8 +1934,8 @@
       <c r="S14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1975,7 +1975,7 @@
         <f t="shared" si="4"/>
         <v>2314.7367225193411</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="8"/>
       <c r="N15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1991,16 +1991,16 @@
       <c r="R15" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
     </row>
     <row r="16" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>SUM(A3:A15)</f>
         <v>768</v>
       </c>
-      <c r="M16" s="15"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="6" t="s">
         <v>64</v>
       </c>
@@ -2355,41 +2355,41 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59">
-        <v>3.56</v>
+        <v>4.76</v>
       </c>
       <c r="D59">
-        <v>5.78</v>
+        <v>15.38</v>
       </c>
       <c r="E59">
-        <v>3.66</v>
+        <v>0.73</v>
       </c>
       <c r="F59">
-        <v>0.56999999999999995</v>
+        <v>8.41</v>
       </c>
       <c r="G59">
-        <v>4.9000000000000002E-2</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61">
         <f>SQRT(2)*C59*2.72^(-0.09/0.05)</f>
-        <v>0.83126782019746892</v>
+        <v>1.1114704562190876</v>
       </c>
       <c r="D61">
         <f t="shared" ref="D61:E61" si="11">SQRT(2)*D59*2.72^(-0.09/0.05)</f>
-        <v>1.3496426968374635</v>
+        <v>3.5912637850104141</v>
       </c>
       <c r="E61">
         <f t="shared" si="11"/>
-        <v>0.85461803986593721</v>
+        <v>0.17045660357981807</v>
       </c>
       <c r="F61">
         <f>SQRT(2)*F59*2.72^(-0.09/0.14)</f>
-        <v>0.42366650438571996</v>
+        <v>6.2509391261121143</v>
       </c>
       <c r="G61">
         <f>SQRT(2)*G59*2.72^(-0.09/0.14)</f>
-        <v>3.6420453885789961E-2</v>
+        <v>0.23041511642030385</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -2398,27 +2398,27 @@
       </c>
       <c r="C63">
         <f>SQRT(2)*C59*(1+2.72^(0.01/0.05))</f>
-        <v>11.18465212299717</v>
+        <v>14.954759580187227</v>
       </c>
       <c r="D63">
         <f t="shared" ref="D63:E63" si="12">SQRT(2)*D59*(1+2.72^(0.01/0.05))</f>
-        <v>18.159350918798776</v>
+        <v>48.320210576319241</v>
       </c>
       <c r="E63">
         <f t="shared" si="12"/>
-        <v>11.498827744429676</v>
+        <v>2.2934820364572848</v>
       </c>
       <c r="F63">
-        <f>SQRT(2)*F59*(1+2.72^(0.01/0.14))</f>
-        <v>1.6719274641015331</v>
+        <f>SQRT(2)*F59*(1+2.72^(0.01/0.246))</f>
+        <v>24.280828661149297</v>
       </c>
       <c r="G63">
-        <f>SQRT(2)*G59*(1+2.72^(0.01/0.14))</f>
-        <v>0.14372709779118442</v>
+        <f>SQRT(2)*G59*(1+2.72^(0.01/0.246))</f>
+        <v>0.89501270926947463</v>
       </c>
       <c r="H63">
         <f>SUM(C63:G63)</f>
-        <v>42.65848534811834</v>
+        <v>90.744293563382541</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -2535,188 +2535,24 @@
         <v>42.60550966494209</v>
       </c>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C76">
-        <f>SQRT(2)*C72*(1+2.72^(0.01/0.05))</f>
-        <v>41.188423969801377</v>
-      </c>
-      <c r="D76">
-        <f t="shared" ref="D76" si="15">SQRT(2)*D72*(1+2.72^(0.01/0.05))</f>
-        <v>5.1838977536363284</v>
-      </c>
-      <c r="E76">
-        <f>SQRT(2)*E72*(1+2.72^(0.01/0.05))</f>
-        <v>5.1838977536363284</v>
-      </c>
-      <c r="F76">
-        <f>SQRT(2)*F72*(1+2.72^(0.01/0.246))</f>
-        <v>0.27427808832451644</v>
-      </c>
-      <c r="G76">
-        <f>SQRT(2)*G72*(1+2.72^(0.01/0.246))</f>
-        <v>0.27427808832451644</v>
-      </c>
-      <c r="H76">
-        <f>SUM(C76:G76)</f>
-        <v>52.104775653723067</v>
-      </c>
-    </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C78">
-        <v>3.44</v>
-      </c>
-      <c r="D78">
-        <v>12.13</v>
-      </c>
-      <c r="E78">
-        <v>4.04</v>
-      </c>
-      <c r="F78">
-        <v>3.46</v>
-      </c>
-      <c r="G78">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C80">
-        <f>SQRT(2)*C78*2.72^(-0.09/0.05)</f>
-        <v>0.80324755659530711</v>
-      </c>
-      <c r="D80">
-        <f t="shared" ref="D80:G80" si="16">SQRT(2)*D78*2.72^(-0.09/0.05)</f>
-        <v>2.8323816457851962</v>
-      </c>
-      <c r="E80">
-        <f t="shared" si="16"/>
-        <v>0.94334887460611649</v>
-      </c>
-      <c r="F80">
-        <f>SQRT(2)*F78*2.72^(-0.09/0.14)</f>
-        <v>2.5717300090782302</v>
-      </c>
-      <c r="G80">
-        <f>SQRT(2)*G78*2.72^(-0.09/0.14)</f>
-        <v>1.2709995131571601</v>
-      </c>
-      <c r="H80">
-        <f>SUM(C80:G80)</f>
-        <v>8.4217075992220103</v>
-      </c>
-    </row>
-    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C82">
-        <f>SQRT(2)*C78*(1+2.72^(0.01/0.05))</f>
-        <v>10.807641377278165</v>
-      </c>
-      <c r="D82">
-        <f t="shared" ref="D82:E82" si="17">SQRT(2)*D78*(1+2.72^(0.01/0.05))</f>
-        <v>38.109502879762836</v>
-      </c>
-      <c r="E82">
-        <f t="shared" si="17"/>
-        <v>12.692695105873193</v>
-      </c>
-      <c r="F82">
-        <f>SQRT(2)*F78*(1+2.72^(0.01/0.14))</f>
-        <v>10.148893027704045</v>
-      </c>
-      <c r="G82">
-        <f>SQRT(2)*G78*(1+2.72^(0.01/0.14))</f>
-        <v>5.0157823923045992</v>
-      </c>
-      <c r="H82">
-        <f>SUM(C82:G82)</f>
-        <v>76.774514782922836</v>
-      </c>
-    </row>
-    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84">
-        <v>3.44</v>
-      </c>
-      <c r="D84">
-        <v>12.13</v>
-      </c>
-      <c r="E84">
-        <v>4.04</v>
-      </c>
-      <c r="F84">
-        <v>3.46</v>
-      </c>
-      <c r="G84">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C86">
-        <f>SQRT(2)*C84*2.72^(0.01/0.05)</f>
-        <v>5.9427467227147188</v>
-      </c>
-      <c r="D86">
-        <f t="shared" ref="D86:E86" si="18">SQRT(2)*D84*2.72^(0.01/0.05)</f>
-        <v>20.955092368177191</v>
-      </c>
-      <c r="E86">
-        <f t="shared" si="18"/>
-        <v>6.9792723138858905</v>
-      </c>
-      <c r="F86">
-        <f>SQRT(2)*F84*2.72^(0.01/0.14)</f>
-        <v>5.2557141018931333</v>
-      </c>
-      <c r="G86">
-        <f>SQRT(2)*G84*2.72^(0.01/0.14)</f>
-        <v>2.597477200646606</v>
-      </c>
-      <c r="H86">
-        <f>SUM(C86:G86)</f>
-        <v>41.730302707317541</v>
-      </c>
-    </row>
-    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C88">
-        <f>SQRT(2)*C84*(1+2.72^(0.01/0.05))</f>
-        <v>10.807641377278165</v>
-      </c>
-      <c r="D88">
-        <f t="shared" ref="D88:E88" si="19">SQRT(2)*D84*(1+2.72^(0.01/0.05))</f>
-        <v>38.109502879762836</v>
-      </c>
-      <c r="E88">
-        <f t="shared" si="19"/>
-        <v>12.692695105873193</v>
-      </c>
-      <c r="F88">
-        <f>SQRT(2)*F84*(1+2.72^(0.01/0.14))</f>
-        <v>10.148893027704045</v>
-      </c>
-      <c r="G88">
-        <f>SQRT(2)*G84*(1+2.72^(0.01/0.14))</f>
-        <v>5.0157823923045992</v>
-      </c>
-      <c r="H88">
-        <f>SUM(C88:G88)</f>
-        <v>76.774514782922836</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="M5:M10"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T5:T9"/>
-    <mergeCell ref="U5:U9"/>
-    <mergeCell ref="M11:M16"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="T11:T15"/>
-    <mergeCell ref="U11:U15"/>
-    <mergeCell ref="S14:S15"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
+    <mergeCell ref="M11:M16"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="T11:T15"/>
+    <mergeCell ref="U11:U15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="M5:M10"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T5:T9"/>
+    <mergeCell ref="U5:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>